<commit_message>
Formatando a Data na coluna 0 para o formato dd/MM/YYYY
</commit_message>
<xml_diff>
--- a/analise/operadoras.xlsx
+++ b/analise/operadoras.xlsx
@@ -77,7 +77,7 @@
     <t>OUTROS</t>
   </si>
   <si>
-    <t>2024-08-23</t>
+    <t>23/08/2024</t>
   </si>
   <si>
     <t>ope014</t>
@@ -2745,7 +2745,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.3046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.65625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="12.8046875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="8.90625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="8.90625" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Mesclando a coluna de totais e medias
</commit_message>
<xml_diff>
--- a/analise/operadoras.xlsx
+++ b/analise/operadoras.xlsx
@@ -1382,7 +1382,7 @@
     <t>1 - 00:21:19</t>
   </si>
   <si>
-    <t>Total de Agentes</t>
+    <t>Total OPE</t>
   </si>
   <si>
     <t>Total Geral</t>
@@ -1397,10 +1397,10 @@
     <t>03:49:19</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Média Geral</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>02:01:42</t>
@@ -4913,14 +4913,14 @@
       <c r="A36" t="s" s="1">
         <v>456</v>
       </c>
-      <c r="B36" t="s" s="1">
+      <c r="B36" t="n" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="C36" t="s" s="1">
+        <v>457</v>
+      </c>
+      <c r="D36" t="s" s="1">
         <v>14</v>
-      </c>
-      <c r="C36" t="n" s="1">
-        <v>33.0</v>
-      </c>
-      <c r="D36" t="s" s="1">
-        <v>457</v>
       </c>
       <c r="E36" t="s" s="1">
         <v>14</v>
@@ -4955,22 +4955,22 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="1">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s" s="1">
         <v>461</v>
-      </c>
-      <c r="B37" t="s" s="1">
-        <v>462</v>
       </c>
       <c r="C37" t="s" s="1">
         <v>462</v>
       </c>
       <c r="D37" t="s" s="1">
-        <v>462</v>
+        <v>14</v>
       </c>
       <c r="E37" t="s" s="1">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F37" t="s" s="1">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H37" t="n" s="1">
         <v>302.0</v>
@@ -4995,9 +4995,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A37:H37"/>
+  <mergeCells count="4">
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C37:H37"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
criando a tabela de indice e formatando
</commit_message>
<xml_diff>
--- a/analise/operadoras.xlsx
+++ b/analise/operadoras.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="440">
   <si>
     <t>DATA</t>
   </si>
@@ -1260,6 +1260,78 @@
   </si>
   <si>
     <t>01:57:58</t>
+  </si>
+  <si>
+    <t>TABELA DE INDICE</t>
+  </si>
+  <si>
+    <t>1º LIGAÇÃO</t>
+  </si>
+  <si>
+    <t>1º L</t>
+  </si>
+  <si>
+    <t>09:05:59</t>
+  </si>
+  <si>
+    <t>JORNADA DE TRABALHO DIÁRIA</t>
+  </si>
+  <si>
+    <t>06:00:00</t>
+  </si>
+  <si>
+    <t>TEMPO LOGADO</t>
+  </si>
+  <si>
+    <t>TOTAL DE HORAS TRABALHA NA PA</t>
+  </si>
+  <si>
+    <t>THPA</t>
+  </si>
+  <si>
+    <t>05:20:00</t>
+  </si>
+  <si>
+    <t>TEMPO TOTAL EM LIGAÇÃO</t>
+  </si>
+  <si>
+    <t>03:10:00</t>
+  </si>
+  <si>
+    <t>QUANTIDADE DE LIGAÇÕES</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>TEMPO MEDIO ATENDIMENTO</t>
+  </si>
+  <si>
+    <t>00:00:40</t>
+  </si>
+  <si>
+    <t>MAIOR TEMPO EM UMA SÓ LIGAÇÃO</t>
+  </si>
+  <si>
+    <t>00:03:00</t>
+  </si>
+  <si>
+    <t>REFERÊNCIA DE TEMPO DE LIGAÇÃO</t>
+  </si>
+  <si>
+    <t>RTL</t>
+  </si>
+  <si>
+    <t>00:01:30</t>
+  </si>
+  <si>
+    <t>TÉRMINO DA ÚLTIMA LIGAÇÃO DO DIA</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>OUTROS: FEEDBACK, MANUTENÇÃO, REUNIÃO E TREINAMENTO</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1339,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="110">
+  <fonts count="111">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -1277,6 +1349,11 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <sz val="11.0"/>
       <b val="true"/>
       <color indexed="9"/>
@@ -1901,12 +1978,32 @@
       <color indexed="8"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="55"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="55"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none">
@@ -1959,13 +2056,81 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <right style="thin"/>
+    </border>
+    <border>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
     </border>
     <border>
       <right style="dashed"/>
@@ -2033,438 +2198,436 @@
         <color indexed="8"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="7" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="9" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="7" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="9" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="59" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="62" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="63" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="64" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="67" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="70" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="73" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="74" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="76" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="79" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="80" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="82" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="83" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="86" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="88" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="89" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="90" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="91" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="92" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="93" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="94" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="95" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="97" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="98" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="99" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="101" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="102" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="103" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="105" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="107" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="108" fillId="11" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="109" fillId="5" borderId="12" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true" applyNumberFormat="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" xfId="0" applyFont="true" applyFill="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="13" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="13" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="11" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="13" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="11" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="13" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="15" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="9" borderId="8" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2473,7 +2636,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U47"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2500,1988 +2663,2210 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" t="s" s="6">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" t="s" s="7">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="4">
+      <c r="C1" t="s" s="8">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="5">
+      <c r="D1" t="s" s="9">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="6">
+      <c r="E1" t="s" s="10">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="7">
+      <c r="F1" t="s" s="11">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="8">
+      <c r="G1" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="9">
+      <c r="H1" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="10">
+      <c r="I1" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="11">
+      <c r="J1" t="s" s="15">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="12">
+      <c r="K1" t="s" s="16">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="13">
+      <c r="L1" t="s" s="17">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="14">
+      <c r="M1" t="s" s="18">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="15">
+      <c r="N1" t="s" s="19">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="16">
+      <c r="O1" t="s" s="20">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="17">
+      <c r="P1" t="s" s="21">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="18">
+      <c r="Q1" t="s" s="22">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="19">
+      <c r="R1" t="s" s="23">
         <v>17</v>
       </c>
-      <c r="S1" t="s" s="20">
+      <c r="S1" t="s" s="24">
         <v>18</v>
       </c>
-      <c r="T1" t="s" s="21">
+      <c r="T1" t="s" s="25">
         <v>19</v>
       </c>
-      <c r="U1" t="s" s="22">
+      <c r="U1" t="s" s="26">
         <v>20</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="23">
+      <c r="A2" t="s" s="27">
         <v>21</v>
       </c>
-      <c r="B2" t="s" s="23">
+      <c r="B2" t="s" s="27">
         <v>22</v>
       </c>
-      <c r="C2" t="s" s="23">
+      <c r="C2" t="s" s="27">
         <v>30</v>
       </c>
-      <c r="D2" t="s" s="23">
+      <c r="D2" t="s" s="27">
         <v>31</v>
       </c>
-      <c r="E2" t="s" s="24">
+      <c r="E2" t="s" s="28">
         <v>23</v>
       </c>
-      <c r="F2" t="s" s="23">
+      <c r="F2" t="s" s="27">
         <v>24</v>
       </c>
-      <c r="G2" t="s" s="23">
+      <c r="G2" t="s" s="27">
         <v>32</v>
       </c>
-      <c r="H2" t="s" s="23">
+      <c r="H2" t="s" s="27">
         <v>33</v>
       </c>
-      <c r="I2" t="n" s="81">
+      <c r="I2" t="n" s="85">
         <v>245.0</v>
       </c>
-      <c r="J2" t="s" s="23">
+      <c r="J2" t="s" s="27">
         <v>25</v>
       </c>
-      <c r="K2" t="s" s="82">
+      <c r="K2" t="s" s="86">
         <v>26</v>
       </c>
-      <c r="L2" t="s" s="23">
+      <c r="L2" t="s" s="27">
         <v>27</v>
       </c>
-      <c r="M2" t="s" s="23">
+      <c r="M2" t="s" s="27">
         <v>28</v>
       </c>
-      <c r="N2" t="s" s="23">
+      <c r="N2" t="s" s="27">
         <v>29</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" t="s" s="23">
+      <c r="O2" s="27"/>
+      <c r="P2" t="s" s="27">
         <v>34</v>
       </c>
-      <c r="Q2" t="s" s="23">
-        <v>35</v>
-      </c>
-      <c r="R2" t="s" s="23">
+      <c r="Q2" t="s" s="27">
+        <v>35</v>
+      </c>
+      <c r="R2" t="s" s="27">
         <v>36</v>
       </c>
-      <c r="S2" t="s" s="23">
-        <v>35</v>
-      </c>
-      <c r="T2" t="s" s="23">
-        <v>35</v>
-      </c>
-      <c r="U2" t="s" s="23">
+      <c r="S2" t="s" s="27">
+        <v>35</v>
+      </c>
+      <c r="T2" t="s" s="27">
+        <v>35</v>
+      </c>
+      <c r="U2" t="s" s="27">
         <v>35</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="25">
+      <c r="A3" t="s" s="29">
         <v>21</v>
       </c>
-      <c r="B3" t="s" s="25">
+      <c r="B3" t="s" s="29">
         <v>37</v>
       </c>
-      <c r="C3" t="s" s="25">
+      <c r="C3" t="s" s="29">
         <v>45</v>
       </c>
-      <c r="D3" t="s" s="25">
+      <c r="D3" t="s" s="29">
         <v>46</v>
       </c>
-      <c r="E3" t="s" s="26">
+      <c r="E3" t="s" s="30">
         <v>38</v>
       </c>
-      <c r="F3" t="s" s="25">
+      <c r="F3" t="s" s="29">
         <v>39</v>
       </c>
-      <c r="G3" t="s" s="25">
+      <c r="G3" t="s" s="29">
         <v>47</v>
       </c>
-      <c r="H3" t="s" s="25">
+      <c r="H3" t="s" s="29">
         <v>48</v>
       </c>
-      <c r="I3" t="n" s="83">
+      <c r="I3" t="n" s="87">
         <v>275.0</v>
       </c>
-      <c r="J3" t="s" s="25">
+      <c r="J3" t="s" s="29">
         <v>40</v>
       </c>
-      <c r="K3" t="s" s="84">
+      <c r="K3" t="s" s="88">
         <v>41</v>
       </c>
-      <c r="L3" t="s" s="25">
+      <c r="L3" t="s" s="29">
         <v>42</v>
       </c>
-      <c r="M3" t="s" s="25">
+      <c r="M3" t="s" s="29">
         <v>43</v>
       </c>
-      <c r="N3" t="s" s="25">
+      <c r="N3" t="s" s="29">
         <v>44</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" t="s" s="25">
+      <c r="O3" s="29"/>
+      <c r="P3" t="s" s="29">
         <v>49</v>
       </c>
-      <c r="Q3" t="s" s="25">
+      <c r="Q3" t="s" s="29">
         <v>50</v>
       </c>
-      <c r="R3" t="s" s="25">
+      <c r="R3" t="s" s="29">
         <v>51</v>
       </c>
-      <c r="S3" t="s" s="25">
-        <v>35</v>
-      </c>
-      <c r="T3" t="s" s="25">
+      <c r="S3" t="s" s="29">
+        <v>35</v>
+      </c>
+      <c r="T3" t="s" s="29">
         <v>52</v>
       </c>
-      <c r="U3" t="s" s="25">
+      <c r="U3" t="s" s="29">
         <v>35</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="27">
+      <c r="A4" t="s" s="31">
         <v>21</v>
       </c>
-      <c r="B4" t="s" s="27">
+      <c r="B4" t="s" s="31">
         <v>53</v>
       </c>
-      <c r="C4" t="s" s="27">
+      <c r="C4" t="s" s="31">
         <v>61</v>
       </c>
-      <c r="D4" t="s" s="27">
+      <c r="D4" t="s" s="31">
         <v>62</v>
       </c>
-      <c r="E4" t="s" s="28">
+      <c r="E4" t="s" s="32">
         <v>54</v>
       </c>
-      <c r="F4" t="s" s="27">
+      <c r="F4" t="s" s="31">
         <v>55</v>
       </c>
-      <c r="G4" t="s" s="27">
+      <c r="G4" t="s" s="31">
         <v>63</v>
       </c>
-      <c r="H4" t="s" s="27">
+      <c r="H4" t="s" s="31">
         <v>64</v>
       </c>
-      <c r="I4" t="n" s="85">
+      <c r="I4" t="n" s="89">
         <v>252.0</v>
       </c>
-      <c r="J4" t="s" s="27">
+      <c r="J4" t="s" s="31">
         <v>56</v>
       </c>
-      <c r="K4" t="s" s="86">
+      <c r="K4" t="s" s="90">
         <v>57</v>
       </c>
-      <c r="L4" t="s" s="27">
+      <c r="L4" t="s" s="31">
         <v>58</v>
       </c>
-      <c r="M4" t="s" s="27">
+      <c r="M4" t="s" s="31">
         <v>59</v>
       </c>
-      <c r="N4" t="s" s="27">
+      <c r="N4" t="s" s="31">
         <v>60</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" t="s" s="27">
+      <c r="O4" s="31"/>
+      <c r="P4" t="s" s="31">
         <v>65</v>
       </c>
-      <c r="Q4" t="s" s="27">
+      <c r="Q4" t="s" s="31">
         <v>66</v>
       </c>
-      <c r="R4" t="s" s="27">
+      <c r="R4" t="s" s="31">
         <v>67</v>
       </c>
-      <c r="S4" t="s" s="27">
-        <v>35</v>
-      </c>
-      <c r="T4" t="s" s="27">
-        <v>35</v>
-      </c>
-      <c r="U4" t="s" s="27">
+      <c r="S4" t="s" s="31">
+        <v>35</v>
+      </c>
+      <c r="T4" t="s" s="31">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s" s="31">
         <v>35</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="29">
+      <c r="A5" t="s" s="33">
         <v>21</v>
       </c>
-      <c r="B5" t="s" s="29">
+      <c r="B5" t="s" s="33">
         <v>68</v>
       </c>
-      <c r="C5" t="s" s="29">
+      <c r="C5" t="s" s="33">
         <v>75</v>
       </c>
-      <c r="D5" t="s" s="29">
+      <c r="D5" t="s" s="33">
         <v>76</v>
       </c>
-      <c r="E5" t="s" s="30">
+      <c r="E5" t="s" s="34">
         <v>69</v>
       </c>
-      <c r="F5" t="s" s="29">
+      <c r="F5" t="s" s="33">
         <v>70</v>
       </c>
-      <c r="G5" t="s" s="29">
+      <c r="G5" t="s" s="33">
         <v>77</v>
       </c>
-      <c r="H5" t="s" s="29">
+      <c r="H5" t="s" s="33">
         <v>78</v>
       </c>
-      <c r="I5" t="n" s="87">
+      <c r="I5" t="n" s="91">
         <v>284.0</v>
       </c>
-      <c r="J5" t="s" s="29">
+      <c r="J5" t="s" s="33">
         <v>71</v>
       </c>
-      <c r="K5" t="s" s="88">
+      <c r="K5" t="s" s="92">
         <v>72</v>
       </c>
-      <c r="L5" t="s" s="29">
+      <c r="L5" t="s" s="33">
         <v>73</v>
       </c>
-      <c r="M5" t="s" s="29">
+      <c r="M5" t="s" s="33">
         <v>74</v>
       </c>
-      <c r="N5" t="s" s="29">
+      <c r="N5" t="s" s="33">
         <v>44</v>
       </c>
-      <c r="O5" s="29"/>
-      <c r="P5" t="s" s="29">
+      <c r="O5" s="33"/>
+      <c r="P5" t="s" s="33">
         <v>79</v>
       </c>
-      <c r="Q5" t="s" s="29">
+      <c r="Q5" t="s" s="33">
         <v>80</v>
       </c>
-      <c r="R5" t="s" s="29">
+      <c r="R5" t="s" s="33">
         <v>81</v>
       </c>
-      <c r="S5" t="s" s="29">
-        <v>35</v>
-      </c>
-      <c r="T5" t="s" s="29">
-        <v>35</v>
-      </c>
-      <c r="U5" t="s" s="29">
+      <c r="S5" t="s" s="33">
+        <v>35</v>
+      </c>
+      <c r="T5" t="s" s="33">
+        <v>35</v>
+      </c>
+      <c r="U5" t="s" s="33">
         <v>35</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="31">
+      <c r="A6" t="s" s="35">
         <v>21</v>
       </c>
-      <c r="B6" t="s" s="31">
+      <c r="B6" t="s" s="35">
         <v>82</v>
       </c>
-      <c r="C6" t="s" s="31">
+      <c r="C6" t="s" s="35">
         <v>89</v>
       </c>
-      <c r="D6" t="s" s="31">
+      <c r="D6" t="s" s="35">
         <v>90</v>
       </c>
-      <c r="E6" t="s" s="32">
+      <c r="E6" t="s" s="36">
         <v>83</v>
       </c>
-      <c r="F6" t="s" s="31">
+      <c r="F6" t="s" s="35">
         <v>84</v>
       </c>
-      <c r="G6" t="s" s="31">
+      <c r="G6" t="s" s="35">
         <v>91</v>
       </c>
-      <c r="H6" t="s" s="31">
+      <c r="H6" t="s" s="35">
         <v>92</v>
       </c>
-      <c r="I6" t="n" s="89">
+      <c r="I6" t="n" s="93">
         <v>167.0</v>
       </c>
-      <c r="J6" t="s" s="31">
+      <c r="J6" t="s" s="35">
         <v>56</v>
       </c>
-      <c r="K6" t="s" s="90">
+      <c r="K6" t="s" s="94">
         <v>85</v>
       </c>
-      <c r="L6" t="s" s="31">
+      <c r="L6" t="s" s="35">
         <v>86</v>
       </c>
-      <c r="M6" t="s" s="31">
+      <c r="M6" t="s" s="35">
         <v>87</v>
       </c>
-      <c r="N6" t="s" s="31">
+      <c r="N6" t="s" s="35">
         <v>88</v>
       </c>
-      <c r="O6" s="31"/>
-      <c r="P6" t="s" s="31">
+      <c r="O6" s="35"/>
+      <c r="P6" t="s" s="35">
         <v>93</v>
       </c>
-      <c r="Q6" t="s" s="31">
+      <c r="Q6" t="s" s="35">
         <v>94</v>
       </c>
-      <c r="R6" t="s" s="31">
+      <c r="R6" t="s" s="35">
         <v>95</v>
       </c>
-      <c r="S6" t="s" s="31">
-        <v>35</v>
-      </c>
-      <c r="T6" t="s" s="31">
-        <v>35</v>
-      </c>
-      <c r="U6" t="s" s="31">
+      <c r="S6" t="s" s="35">
+        <v>35</v>
+      </c>
+      <c r="T6" t="s" s="35">
+        <v>35</v>
+      </c>
+      <c r="U6" t="s" s="35">
         <v>35</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="33">
+      <c r="A7" t="s" s="37">
         <v>21</v>
       </c>
-      <c r="B7" t="s" s="33">
+      <c r="B7" t="s" s="37">
         <v>96</v>
       </c>
-      <c r="C7" t="s" s="33">
+      <c r="C7" t="s" s="37">
         <v>103</v>
       </c>
-      <c r="D7" t="s" s="33">
+      <c r="D7" t="s" s="37">
         <v>104</v>
       </c>
-      <c r="E7" t="s" s="34">
+      <c r="E7" t="s" s="38">
         <v>38</v>
       </c>
-      <c r="F7" t="s" s="33">
+      <c r="F7" t="s" s="37">
         <v>97</v>
       </c>
-      <c r="G7" t="s" s="33">
+      <c r="G7" t="s" s="37">
         <v>77</v>
       </c>
-      <c r="H7" t="s" s="33">
+      <c r="H7" t="s" s="37">
         <v>105</v>
       </c>
-      <c r="I7" t="n" s="91">
+      <c r="I7" t="n" s="95">
         <v>265.0</v>
       </c>
-      <c r="J7" t="s" s="33">
+      <c r="J7" t="s" s="37">
         <v>98</v>
       </c>
-      <c r="K7" t="s" s="92">
+      <c r="K7" t="s" s="96">
         <v>99</v>
       </c>
-      <c r="L7" t="s" s="33">
+      <c r="L7" t="s" s="37">
         <v>100</v>
       </c>
-      <c r="M7" t="s" s="33">
+      <c r="M7" t="s" s="37">
         <v>101</v>
       </c>
-      <c r="N7" t="s" s="33">
+      <c r="N7" t="s" s="37">
         <v>102</v>
       </c>
-      <c r="O7" s="33"/>
-      <c r="P7" t="s" s="33">
+      <c r="O7" s="37"/>
+      <c r="P7" t="s" s="37">
         <v>106</v>
       </c>
-      <c r="Q7" t="s" s="33">
-        <v>35</v>
-      </c>
-      <c r="R7" t="s" s="33">
+      <c r="Q7" t="s" s="37">
+        <v>35</v>
+      </c>
+      <c r="R7" t="s" s="37">
         <v>107</v>
       </c>
-      <c r="S7" t="s" s="33">
-        <v>35</v>
-      </c>
-      <c r="T7" t="s" s="33">
+      <c r="S7" t="s" s="37">
+        <v>35</v>
+      </c>
+      <c r="T7" t="s" s="37">
         <v>108</v>
       </c>
-      <c r="U7" t="s" s="33">
+      <c r="U7" t="s" s="37">
         <v>109</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="35">
+      <c r="A8" t="s" s="39">
         <v>21</v>
       </c>
-      <c r="B8" t="s" s="35">
+      <c r="B8" t="s" s="39">
         <v>110</v>
       </c>
-      <c r="C8" t="s" s="35">
+      <c r="C8" t="s" s="39">
         <v>117</v>
       </c>
-      <c r="D8" t="s" s="35">
+      <c r="D8" t="s" s="39">
         <v>118</v>
       </c>
-      <c r="E8" t="s" s="36">
+      <c r="E8" t="s" s="40">
         <v>111</v>
       </c>
-      <c r="F8" t="s" s="35">
+      <c r="F8" t="s" s="39">
         <v>112</v>
       </c>
-      <c r="G8" t="s" s="35">
+      <c r="G8" t="s" s="39">
         <v>119</v>
       </c>
-      <c r="H8" t="s" s="35">
+      <c r="H8" t="s" s="39">
         <v>120</v>
       </c>
-      <c r="I8" t="n" s="93">
+      <c r="I8" t="n" s="97">
         <v>273.0</v>
       </c>
-      <c r="J8" t="s" s="35">
+      <c r="J8" t="s" s="39">
         <v>113</v>
       </c>
-      <c r="K8" t="s" s="94">
+      <c r="K8" t="s" s="98">
         <v>114</v>
       </c>
-      <c r="L8" t="s" s="35">
+      <c r="L8" t="s" s="39">
         <v>115</v>
       </c>
-      <c r="M8" t="s" s="35">
+      <c r="M8" t="s" s="39">
         <v>59</v>
       </c>
-      <c r="N8" t="s" s="35">
+      <c r="N8" t="s" s="39">
         <v>116</v>
       </c>
-      <c r="O8" s="35"/>
-      <c r="P8" t="s" s="35">
+      <c r="O8" s="39"/>
+      <c r="P8" t="s" s="39">
         <v>121</v>
       </c>
-      <c r="Q8" t="s" s="35">
+      <c r="Q8" t="s" s="39">
         <v>80</v>
       </c>
-      <c r="R8" t="s" s="35">
+      <c r="R8" t="s" s="39">
         <v>122</v>
       </c>
-      <c r="S8" t="s" s="35">
-        <v>35</v>
-      </c>
-      <c r="T8" t="s" s="35">
-        <v>35</v>
-      </c>
-      <c r="U8" t="s" s="35">
+      <c r="S8" t="s" s="39">
+        <v>35</v>
+      </c>
+      <c r="T8" t="s" s="39">
+        <v>35</v>
+      </c>
+      <c r="U8" t="s" s="39">
         <v>35</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="37">
+      <c r="A9" t="s" s="41">
         <v>21</v>
       </c>
-      <c r="B9" t="s" s="37">
+      <c r="B9" t="s" s="41">
         <v>123</v>
       </c>
-      <c r="C9" t="s" s="37">
+      <c r="C9" t="s" s="41">
         <v>75</v>
       </c>
-      <c r="D9" t="s" s="37">
+      <c r="D9" t="s" s="41">
         <v>129</v>
       </c>
-      <c r="E9" t="s" s="38">
+      <c r="E9" t="s" s="42">
         <v>124</v>
       </c>
-      <c r="F9" t="s" s="37">
+      <c r="F9" t="s" s="41">
         <v>125</v>
       </c>
-      <c r="G9" t="s" s="37">
+      <c r="G9" t="s" s="41">
         <v>130</v>
       </c>
-      <c r="H9" t="s" s="37">
+      <c r="H9" t="s" s="41">
         <v>131</v>
       </c>
-      <c r="I9" t="n" s="95">
+      <c r="I9" t="n" s="99">
         <v>275.0</v>
       </c>
-      <c r="J9" t="s" s="37">
+      <c r="J9" t="s" s="41">
         <v>113</v>
       </c>
-      <c r="K9" t="s" s="96">
+      <c r="K9" t="s" s="100">
         <v>126</v>
       </c>
-      <c r="L9" t="s" s="37">
+      <c r="L9" t="s" s="41">
         <v>127</v>
       </c>
-      <c r="M9" t="s" s="37">
+      <c r="M9" t="s" s="41">
         <v>59</v>
       </c>
-      <c r="N9" t="s" s="37">
+      <c r="N9" t="s" s="41">
         <v>128</v>
       </c>
-      <c r="O9" s="37"/>
-      <c r="P9" t="s" s="37">
+      <c r="O9" s="41"/>
+      <c r="P9" t="s" s="41">
         <v>132</v>
       </c>
-      <c r="Q9" t="s" s="37">
+      <c r="Q9" t="s" s="41">
         <v>133</v>
       </c>
-      <c r="R9" t="s" s="37">
+      <c r="R9" t="s" s="41">
         <v>134</v>
       </c>
-      <c r="S9" t="s" s="37">
-        <v>35</v>
-      </c>
-      <c r="T9" t="s" s="37">
-        <v>35</v>
-      </c>
-      <c r="U9" t="s" s="37">
+      <c r="S9" t="s" s="41">
+        <v>35</v>
+      </c>
+      <c r="T9" t="s" s="41">
+        <v>35</v>
+      </c>
+      <c r="U9" t="s" s="41">
         <v>35</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="39">
+      <c r="A10" t="s" s="43">
         <v>21</v>
       </c>
-      <c r="B10" t="s" s="39">
+      <c r="B10" t="s" s="43">
         <v>135</v>
       </c>
-      <c r="C10" t="s" s="39">
+      <c r="C10" t="s" s="43">
         <v>139</v>
       </c>
-      <c r="D10" t="s" s="39">
+      <c r="D10" t="s" s="43">
         <v>140</v>
       </c>
-      <c r="E10" t="s" s="40">
+      <c r="E10" t="s" s="44">
         <v>124</v>
       </c>
-      <c r="F10" t="s" s="39">
+      <c r="F10" t="s" s="43">
         <v>136</v>
       </c>
-      <c r="G10" t="s" s="39">
+      <c r="G10" t="s" s="43">
         <v>141</v>
       </c>
-      <c r="H10" t="s" s="39">
+      <c r="H10" t="s" s="43">
         <v>142</v>
       </c>
-      <c r="I10" t="n" s="97">
+      <c r="I10" t="n" s="101">
         <v>258.0</v>
       </c>
-      <c r="J10" t="s" s="39">
+      <c r="J10" t="s" s="43">
         <v>56</v>
       </c>
-      <c r="K10" t="s" s="98">
+      <c r="K10" t="s" s="102">
         <v>137</v>
       </c>
-      <c r="L10" t="s" s="39">
+      <c r="L10" t="s" s="43">
         <v>86</v>
       </c>
-      <c r="M10" t="s" s="39">
+      <c r="M10" t="s" s="43">
         <v>101</v>
       </c>
-      <c r="N10" t="s" s="39">
+      <c r="N10" t="s" s="43">
         <v>138</v>
       </c>
-      <c r="O10" s="39"/>
-      <c r="P10" t="s" s="39">
+      <c r="O10" s="43"/>
+      <c r="P10" t="s" s="43">
         <v>143</v>
       </c>
-      <c r="Q10" t="s" s="39">
+      <c r="Q10" t="s" s="43">
         <v>144</v>
       </c>
-      <c r="R10" t="s" s="39">
+      <c r="R10" t="s" s="43">
         <v>145</v>
       </c>
-      <c r="S10" t="s" s="39">
-        <v>35</v>
-      </c>
-      <c r="T10" t="s" s="39">
-        <v>35</v>
-      </c>
-      <c r="U10" t="s" s="39">
+      <c r="S10" t="s" s="43">
+        <v>35</v>
+      </c>
+      <c r="T10" t="s" s="43">
+        <v>35</v>
+      </c>
+      <c r="U10" t="s" s="43">
         <v>35</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="41">
+      <c r="A11" t="s" s="45">
         <v>21</v>
       </c>
-      <c r="B11" t="s" s="41">
+      <c r="B11" t="s" s="45">
         <v>146</v>
       </c>
-      <c r="C11" t="s" s="41">
+      <c r="C11" t="s" s="45">
         <v>154</v>
       </c>
-      <c r="D11" t="s" s="41">
+      <c r="D11" t="s" s="45">
         <v>155</v>
       </c>
-      <c r="E11" t="s" s="42">
+      <c r="E11" t="s" s="46">
         <v>147</v>
       </c>
-      <c r="F11" t="s" s="41">
+      <c r="F11" t="s" s="45">
         <v>148</v>
       </c>
-      <c r="G11" t="s" s="41">
+      <c r="G11" t="s" s="45">
         <v>156</v>
       </c>
-      <c r="H11" t="s" s="41">
+      <c r="H11" t="s" s="45">
         <v>157</v>
       </c>
-      <c r="I11" t="n" s="99">
+      <c r="I11" t="n" s="103">
         <v>312.0</v>
       </c>
-      <c r="J11" t="s" s="41">
+      <c r="J11" t="s" s="45">
         <v>149</v>
       </c>
-      <c r="K11" t="s" s="100">
+      <c r="K11" t="s" s="104">
         <v>150</v>
       </c>
-      <c r="L11" t="s" s="41">
+      <c r="L11" t="s" s="45">
         <v>151</v>
       </c>
-      <c r="M11" t="s" s="41">
+      <c r="M11" t="s" s="45">
         <v>152</v>
       </c>
-      <c r="N11" t="s" s="41">
+      <c r="N11" t="s" s="45">
         <v>153</v>
       </c>
-      <c r="O11" s="41"/>
-      <c r="P11" t="s" s="41">
+      <c r="O11" s="45"/>
+      <c r="P11" t="s" s="45">
         <v>158</v>
       </c>
-      <c r="Q11" t="s" s="41">
+      <c r="Q11" t="s" s="45">
         <v>159</v>
       </c>
-      <c r="R11" t="s" s="41">
+      <c r="R11" t="s" s="45">
         <v>160</v>
       </c>
-      <c r="S11" t="s" s="41">
-        <v>35</v>
-      </c>
-      <c r="T11" t="s" s="41">
-        <v>35</v>
-      </c>
-      <c r="U11" t="s" s="41">
+      <c r="S11" t="s" s="45">
+        <v>35</v>
+      </c>
+      <c r="T11" t="s" s="45">
+        <v>35</v>
+      </c>
+      <c r="U11" t="s" s="45">
         <v>35</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s" s="43">
+      <c r="A12" t="s" s="47">
         <v>21</v>
       </c>
-      <c r="B12" t="s" s="43">
+      <c r="B12" t="s" s="47">
         <v>161</v>
       </c>
-      <c r="C12" t="s" s="43">
+      <c r="C12" t="s" s="47">
         <v>168</v>
       </c>
-      <c r="D12" t="s" s="43">
+      <c r="D12" t="s" s="47">
         <v>169</v>
       </c>
-      <c r="E12" t="s" s="44">
+      <c r="E12" t="s" s="48">
         <v>162</v>
       </c>
-      <c r="F12" t="s" s="43">
+      <c r="F12" t="s" s="47">
         <v>163</v>
       </c>
-      <c r="G12" t="s" s="43">
+      <c r="G12" t="s" s="47">
         <v>170</v>
       </c>
-      <c r="H12" t="s" s="43">
+      <c r="H12" t="s" s="47">
         <v>171</v>
       </c>
-      <c r="I12" t="n" s="101">
+      <c r="I12" t="n" s="105">
         <v>325.0</v>
       </c>
-      <c r="J12" t="s" s="43">
+      <c r="J12" t="s" s="47">
         <v>25</v>
       </c>
-      <c r="K12" t="s" s="102">
+      <c r="K12" t="s" s="106">
         <v>164</v>
       </c>
-      <c r="L12" t="s" s="43">
+      <c r="L12" t="s" s="47">
         <v>165</v>
       </c>
-      <c r="M12" t="s" s="43">
+      <c r="M12" t="s" s="47">
         <v>166</v>
       </c>
-      <c r="N12" t="s" s="43">
+      <c r="N12" t="s" s="47">
         <v>167</v>
       </c>
-      <c r="O12" s="43"/>
-      <c r="P12" t="s" s="43">
+      <c r="O12" s="47"/>
+      <c r="P12" t="s" s="47">
         <v>172</v>
       </c>
-      <c r="Q12" t="s" s="43">
+      <c r="Q12" t="s" s="47">
         <v>173</v>
       </c>
-      <c r="R12" t="s" s="43">
+      <c r="R12" t="s" s="47">
         <v>174</v>
       </c>
-      <c r="S12" t="s" s="43">
-        <v>35</v>
-      </c>
-      <c r="T12" t="s" s="43">
-        <v>35</v>
-      </c>
-      <c r="U12" t="s" s="43">
+      <c r="S12" t="s" s="47">
+        <v>35</v>
+      </c>
+      <c r="T12" t="s" s="47">
+        <v>35</v>
+      </c>
+      <c r="U12" t="s" s="47">
         <v>35</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="45">
+      <c r="A13" t="s" s="49">
         <v>21</v>
       </c>
-      <c r="B13" t="s" s="45">
+      <c r="B13" t="s" s="49">
         <v>175</v>
       </c>
-      <c r="C13" t="s" s="45">
+      <c r="C13" t="s" s="49">
         <v>183</v>
       </c>
-      <c r="D13" t="s" s="45">
+      <c r="D13" t="s" s="49">
         <v>184</v>
       </c>
-      <c r="E13" t="s" s="46">
+      <c r="E13" t="s" s="50">
         <v>176</v>
       </c>
-      <c r="F13" t="s" s="45">
+      <c r="F13" t="s" s="49">
         <v>177</v>
       </c>
-      <c r="G13" t="s" s="45">
+      <c r="G13" t="s" s="49">
         <v>185</v>
       </c>
-      <c r="H13" t="s" s="45">
+      <c r="H13" t="s" s="49">
         <v>186</v>
       </c>
-      <c r="I13" t="n" s="103">
+      <c r="I13" t="n" s="107">
         <v>265.0</v>
       </c>
-      <c r="J13" t="s" s="45">
+      <c r="J13" t="s" s="49">
         <v>178</v>
       </c>
-      <c r="K13" t="s" s="104">
+      <c r="K13" t="s" s="108">
         <v>179</v>
       </c>
-      <c r="L13" t="s" s="45">
+      <c r="L13" t="s" s="49">
         <v>180</v>
       </c>
-      <c r="M13" t="s" s="45">
+      <c r="M13" t="s" s="49">
         <v>181</v>
       </c>
-      <c r="N13" t="s" s="45">
+      <c r="N13" t="s" s="49">
         <v>182</v>
       </c>
-      <c r="O13" s="45"/>
-      <c r="P13" t="s" s="45">
+      <c r="O13" s="49"/>
+      <c r="P13" t="s" s="49">
         <v>187</v>
       </c>
-      <c r="Q13" t="s" s="45">
-        <v>35</v>
-      </c>
-      <c r="R13" t="s" s="45">
+      <c r="Q13" t="s" s="49">
+        <v>35</v>
+      </c>
+      <c r="R13" t="s" s="49">
         <v>188</v>
       </c>
-      <c r="S13" t="s" s="45">
-        <v>35</v>
-      </c>
-      <c r="T13" t="s" s="45">
-        <v>35</v>
-      </c>
-      <c r="U13" t="s" s="45">
+      <c r="S13" t="s" s="49">
+        <v>35</v>
+      </c>
+      <c r="T13" t="s" s="49">
+        <v>35</v>
+      </c>
+      <c r="U13" t="s" s="49">
         <v>35</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s" s="47">
+      <c r="A14" t="s" s="51">
         <v>21</v>
       </c>
-      <c r="B14" t="s" s="47">
+      <c r="B14" t="s" s="51">
         <v>189</v>
       </c>
-      <c r="C14" t="s" s="47">
+      <c r="C14" t="s" s="51">
         <v>197</v>
       </c>
-      <c r="D14" t="s" s="47">
+      <c r="D14" t="s" s="51">
         <v>198</v>
       </c>
-      <c r="E14" t="s" s="48">
+      <c r="E14" t="s" s="52">
         <v>190</v>
       </c>
-      <c r="F14" t="s" s="47">
+      <c r="F14" t="s" s="51">
         <v>191</v>
       </c>
-      <c r="G14" t="s" s="47">
+      <c r="G14" t="s" s="51">
         <v>199</v>
       </c>
-      <c r="H14" t="s" s="47">
+      <c r="H14" t="s" s="51">
         <v>200</v>
       </c>
-      <c r="I14" t="n" s="105">
+      <c r="I14" t="n" s="109">
         <v>178.0</v>
       </c>
-      <c r="J14" t="s" s="47">
+      <c r="J14" t="s" s="51">
         <v>192</v>
       </c>
-      <c r="K14" t="s" s="106">
+      <c r="K14" t="s" s="110">
         <v>193</v>
       </c>
-      <c r="L14" t="s" s="47">
+      <c r="L14" t="s" s="51">
         <v>194</v>
       </c>
-      <c r="M14" t="s" s="47">
+      <c r="M14" t="s" s="51">
         <v>195</v>
       </c>
-      <c r="N14" t="s" s="47">
+      <c r="N14" t="s" s="51">
         <v>196</v>
       </c>
-      <c r="O14" s="47"/>
-      <c r="P14" t="s" s="47">
+      <c r="O14" s="51"/>
+      <c r="P14" t="s" s="51">
         <v>201</v>
       </c>
-      <c r="Q14" t="s" s="47">
+      <c r="Q14" t="s" s="51">
         <v>202</v>
       </c>
-      <c r="R14" t="s" s="47">
+      <c r="R14" t="s" s="51">
         <v>203</v>
       </c>
-      <c r="S14" t="s" s="47">
-        <v>35</v>
-      </c>
-      <c r="T14" t="s" s="47">
-        <v>35</v>
-      </c>
-      <c r="U14" t="s" s="47">
+      <c r="S14" t="s" s="51">
+        <v>35</v>
+      </c>
+      <c r="T14" t="s" s="51">
+        <v>35</v>
+      </c>
+      <c r="U14" t="s" s="51">
         <v>35</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s" s="49">
+      <c r="A15" t="s" s="53">
         <v>21</v>
       </c>
-      <c r="B15" t="s" s="49">
+      <c r="B15" t="s" s="53">
         <v>204</v>
       </c>
-      <c r="C15" t="s" s="49">
+      <c r="C15" t="s" s="53">
         <v>209</v>
       </c>
-      <c r="D15" t="s" s="49">
+      <c r="D15" t="s" s="53">
         <v>210</v>
       </c>
-      <c r="E15" t="s" s="50">
+      <c r="E15" t="s" s="54">
         <v>205</v>
       </c>
-      <c r="F15" t="s" s="49">
+      <c r="F15" t="s" s="53">
         <v>206</v>
       </c>
-      <c r="G15" t="s" s="49">
+      <c r="G15" t="s" s="53">
         <v>211</v>
       </c>
-      <c r="H15" t="s" s="49">
+      <c r="H15" t="s" s="53">
         <v>212</v>
       </c>
-      <c r="I15" t="n" s="107">
+      <c r="I15" t="n" s="111">
         <v>298.0</v>
       </c>
-      <c r="J15" t="s" s="49">
+      <c r="J15" t="s" s="53">
         <v>192</v>
       </c>
-      <c r="K15" t="s" s="108">
+      <c r="K15" t="s" s="112">
         <v>207</v>
       </c>
-      <c r="L15" t="s" s="49">
+      <c r="L15" t="s" s="53">
         <v>194</v>
       </c>
-      <c r="M15" t="s" s="49">
+      <c r="M15" t="s" s="53">
         <v>43</v>
       </c>
-      <c r="N15" t="s" s="49">
+      <c r="N15" t="s" s="53">
         <v>208</v>
       </c>
-      <c r="O15" s="49"/>
-      <c r="P15" t="s" s="49">
+      <c r="O15" s="53"/>
+      <c r="P15" t="s" s="53">
         <v>213</v>
       </c>
-      <c r="Q15" t="s" s="49">
+      <c r="Q15" t="s" s="53">
         <v>214</v>
       </c>
-      <c r="R15" t="s" s="49">
+      <c r="R15" t="s" s="53">
         <v>215</v>
       </c>
-      <c r="S15" t="s" s="49">
-        <v>35</v>
-      </c>
-      <c r="T15" t="s" s="49">
-        <v>35</v>
-      </c>
-      <c r="U15" t="s" s="49">
+      <c r="S15" t="s" s="53">
+        <v>35</v>
+      </c>
+      <c r="T15" t="s" s="53">
+        <v>35</v>
+      </c>
+      <c r="U15" t="s" s="53">
         <v>35</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s" s="51">
+      <c r="A16" t="s" s="55">
         <v>21</v>
       </c>
-      <c r="B16" t="s" s="51">
+      <c r="B16" t="s" s="55">
         <v>216</v>
       </c>
-      <c r="C16" t="s" s="51">
+      <c r="C16" t="s" s="55">
         <v>221</v>
       </c>
-      <c r="D16" t="s" s="51">
+      <c r="D16" t="s" s="55">
         <v>222</v>
       </c>
-      <c r="E16" t="s" s="52">
+      <c r="E16" t="s" s="56">
         <v>217</v>
       </c>
-      <c r="F16" t="s" s="51">
+      <c r="F16" t="s" s="55">
         <v>140</v>
       </c>
-      <c r="G16" t="s" s="51">
+      <c r="G16" t="s" s="55">
         <v>223</v>
       </c>
-      <c r="H16" t="s" s="51">
+      <c r="H16" t="s" s="55">
         <v>224</v>
       </c>
-      <c r="I16" t="n" s="109">
+      <c r="I16" t="n" s="113">
         <v>219.0</v>
       </c>
-      <c r="J16" t="s" s="51">
+      <c r="J16" t="s" s="55">
         <v>25</v>
       </c>
-      <c r="K16" t="s" s="110">
+      <c r="K16" t="s" s="114">
         <v>218</v>
       </c>
-      <c r="L16" t="s" s="51">
+      <c r="L16" t="s" s="55">
         <v>165</v>
       </c>
-      <c r="M16" t="s" s="51">
+      <c r="M16" t="s" s="55">
         <v>219</v>
       </c>
-      <c r="N16" t="s" s="51">
+      <c r="N16" t="s" s="55">
         <v>220</v>
       </c>
-      <c r="O16" s="51"/>
-      <c r="P16" t="s" s="51">
+      <c r="O16" s="55"/>
+      <c r="P16" t="s" s="55">
         <v>225</v>
       </c>
-      <c r="Q16" t="s" s="51">
+      <c r="Q16" t="s" s="55">
         <v>226</v>
       </c>
-      <c r="R16" t="s" s="51">
+      <c r="R16" t="s" s="55">
         <v>81</v>
       </c>
-      <c r="S16" t="s" s="51">
-        <v>35</v>
-      </c>
-      <c r="T16" t="s" s="51">
+      <c r="S16" t="s" s="55">
+        <v>35</v>
+      </c>
+      <c r="T16" t="s" s="55">
         <v>227</v>
       </c>
-      <c r="U16" t="s" s="51">
+      <c r="U16" t="s" s="55">
         <v>35</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="53">
+      <c r="A17" t="s" s="57">
         <v>21</v>
       </c>
-      <c r="B17" t="s" s="53">
+      <c r="B17" t="s" s="57">
         <v>228</v>
       </c>
-      <c r="C17" t="s" s="53">
+      <c r="C17" t="s" s="57">
         <v>235</v>
       </c>
-      <c r="D17" t="s" s="53">
+      <c r="D17" t="s" s="57">
         <v>236</v>
       </c>
-      <c r="E17" t="s" s="54">
+      <c r="E17" t="s" s="58">
         <v>229</v>
       </c>
-      <c r="F17" t="s" s="53">
+      <c r="F17" t="s" s="57">
         <v>230</v>
       </c>
-      <c r="G17" t="s" s="53">
+      <c r="G17" t="s" s="57">
         <v>237</v>
       </c>
-      <c r="H17" t="s" s="53">
+      <c r="H17" t="s" s="57">
         <v>238</v>
       </c>
-      <c r="I17" t="n" s="111">
+      <c r="I17" t="n" s="115">
         <v>358.0</v>
       </c>
-      <c r="J17" t="s" s="53">
+      <c r="J17" t="s" s="57">
         <v>231</v>
       </c>
-      <c r="K17" t="s" s="112">
+      <c r="K17" t="s" s="116">
         <v>232</v>
       </c>
-      <c r="L17" t="s" s="53">
+      <c r="L17" t="s" s="57">
         <v>233</v>
       </c>
-      <c r="M17" t="s" s="53">
+      <c r="M17" t="s" s="57">
         <v>101</v>
       </c>
-      <c r="N17" t="s" s="53">
+      <c r="N17" t="s" s="57">
         <v>234</v>
       </c>
-      <c r="O17" s="53"/>
-      <c r="P17" t="s" s="53">
+      <c r="O17" s="57"/>
+      <c r="P17" t="s" s="57">
         <v>239</v>
       </c>
-      <c r="Q17" t="s" s="53">
+      <c r="Q17" t="s" s="57">
         <v>240</v>
       </c>
-      <c r="R17" t="s" s="53">
+      <c r="R17" t="s" s="57">
         <v>241</v>
       </c>
-      <c r="S17" t="s" s="53">
-        <v>35</v>
-      </c>
-      <c r="T17" t="s" s="53">
+      <c r="S17" t="s" s="57">
+        <v>35</v>
+      </c>
+      <c r="T17" t="s" s="57">
         <v>242</v>
       </c>
-      <c r="U17" t="s" s="53">
+      <c r="U17" t="s" s="57">
         <v>35</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s" s="55">
+      <c r="A18" t="s" s="59">
         <v>21</v>
       </c>
-      <c r="B18" t="s" s="55">
+      <c r="B18" t="s" s="59">
         <v>243</v>
       </c>
-      <c r="C18" t="s" s="55">
+      <c r="C18" t="s" s="59">
         <v>247</v>
       </c>
-      <c r="D18" t="s" s="55">
+      <c r="D18" t="s" s="59">
         <v>248</v>
       </c>
-      <c r="E18" t="s" s="56">
+      <c r="E18" t="s" s="60">
         <v>205</v>
       </c>
-      <c r="F18" t="s" s="55">
+      <c r="F18" t="s" s="59">
         <v>244</v>
       </c>
-      <c r="G18" t="s" s="55">
+      <c r="G18" t="s" s="59">
         <v>249</v>
       </c>
-      <c r="H18" t="s" s="55">
+      <c r="H18" t="s" s="59">
         <v>250</v>
       </c>
-      <c r="I18" t="n" s="113">
+      <c r="I18" t="n" s="117">
         <v>276.0</v>
       </c>
-      <c r="J18" t="s" s="55">
+      <c r="J18" t="s" s="59">
         <v>113</v>
       </c>
-      <c r="K18" t="s" s="114">
+      <c r="K18" t="s" s="118">
         <v>245</v>
       </c>
-      <c r="L18" t="s" s="55">
+      <c r="L18" t="s" s="59">
         <v>115</v>
       </c>
-      <c r="M18" t="s" s="55">
+      <c r="M18" t="s" s="59">
         <v>101</v>
       </c>
-      <c r="N18" t="s" s="55">
+      <c r="N18" t="s" s="59">
         <v>246</v>
       </c>
-      <c r="O18" s="55"/>
-      <c r="P18" t="s" s="55">
+      <c r="O18" s="59"/>
+      <c r="P18" t="s" s="59">
         <v>251</v>
       </c>
-      <c r="Q18" t="s" s="55">
+      <c r="Q18" t="s" s="59">
         <v>252</v>
       </c>
-      <c r="R18" t="s" s="55">
+      <c r="R18" t="s" s="59">
         <v>134</v>
       </c>
-      <c r="S18" t="s" s="55">
-        <v>35</v>
-      </c>
-      <c r="T18" t="s" s="55">
-        <v>35</v>
-      </c>
-      <c r="U18" t="s" s="55">
+      <c r="S18" t="s" s="59">
+        <v>35</v>
+      </c>
+      <c r="T18" t="s" s="59">
+        <v>35</v>
+      </c>
+      <c r="U18" t="s" s="59">
         <v>35</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s" s="57">
+      <c r="A19" t="s" s="61">
         <v>21</v>
       </c>
-      <c r="B19" t="s" s="57">
+      <c r="B19" t="s" s="61">
         <v>253</v>
       </c>
-      <c r="C19" t="s" s="57">
+      <c r="C19" t="s" s="61">
         <v>209</v>
       </c>
-      <c r="D19" t="s" s="57">
+      <c r="D19" t="s" s="61">
         <v>76</v>
       </c>
-      <c r="E19" t="s" s="58">
+      <c r="E19" t="s" s="62">
         <v>254</v>
       </c>
-      <c r="F19" t="s" s="57">
+      <c r="F19" t="s" s="61">
         <v>255</v>
       </c>
-      <c r="G19" t="s" s="57">
+      <c r="G19" t="s" s="61">
         <v>258</v>
       </c>
-      <c r="H19" t="s" s="57">
+      <c r="H19" t="s" s="61">
         <v>259</v>
       </c>
-      <c r="I19" t="n" s="115">
+      <c r="I19" t="n" s="119">
         <v>240.0</v>
       </c>
-      <c r="J19" t="s" s="57">
+      <c r="J19" t="s" s="61">
         <v>231</v>
       </c>
-      <c r="K19" t="s" s="116">
+      <c r="K19" t="s" s="120">
         <v>256</v>
       </c>
-      <c r="L19" t="s" s="57">
+      <c r="L19" t="s" s="61">
         <v>233</v>
       </c>
-      <c r="M19" t="s" s="57">
+      <c r="M19" t="s" s="61">
         <v>219</v>
       </c>
-      <c r="N19" t="s" s="57">
+      <c r="N19" t="s" s="61">
         <v>257</v>
       </c>
-      <c r="O19" s="57"/>
-      <c r="P19" t="s" s="57">
+      <c r="O19" s="61"/>
+      <c r="P19" t="s" s="61">
         <v>260</v>
       </c>
-      <c r="Q19" t="s" s="57">
+      <c r="Q19" t="s" s="61">
         <v>261</v>
       </c>
-      <c r="R19" t="s" s="57">
+      <c r="R19" t="s" s="61">
         <v>262</v>
       </c>
-      <c r="S19" t="s" s="57">
-        <v>35</v>
-      </c>
-      <c r="T19" t="s" s="57">
+      <c r="S19" t="s" s="61">
+        <v>35</v>
+      </c>
+      <c r="T19" t="s" s="61">
         <v>263</v>
       </c>
-      <c r="U19" t="s" s="57">
+      <c r="U19" t="s" s="61">
         <v>35</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s" s="59">
+      <c r="A20" t="s" s="63">
         <v>21</v>
       </c>
-      <c r="B20" t="s" s="59">
+      <c r="B20" t="s" s="63">
         <v>264</v>
       </c>
-      <c r="C20" t="s" s="59">
+      <c r="C20" t="s" s="63">
         <v>270</v>
       </c>
-      <c r="D20" t="s" s="59">
+      <c r="D20" t="s" s="63">
         <v>271</v>
       </c>
-      <c r="E20" t="s" s="60">
+      <c r="E20" t="s" s="64">
         <v>265</v>
       </c>
-      <c r="F20" t="s" s="59">
+      <c r="F20" t="s" s="63">
         <v>266</v>
       </c>
-      <c r="G20" t="s" s="59">
+      <c r="G20" t="s" s="63">
         <v>272</v>
       </c>
-      <c r="H20" t="s" s="59">
+      <c r="H20" t="s" s="63">
         <v>273</v>
       </c>
-      <c r="I20" t="n" s="117">
+      <c r="I20" t="n" s="121">
         <v>219.0</v>
       </c>
-      <c r="J20" t="s" s="59">
+      <c r="J20" t="s" s="63">
         <v>56</v>
       </c>
-      <c r="K20" t="s" s="118">
+      <c r="K20" t="s" s="122">
         <v>267</v>
       </c>
-      <c r="L20" t="s" s="59">
+      <c r="L20" t="s" s="63">
         <v>86</v>
       </c>
-      <c r="M20" t="s" s="59">
+      <c r="M20" t="s" s="63">
         <v>268</v>
       </c>
-      <c r="N20" t="s" s="59">
+      <c r="N20" t="s" s="63">
         <v>269</v>
       </c>
-      <c r="O20" s="59"/>
-      <c r="P20" t="s" s="59">
+      <c r="O20" s="63"/>
+      <c r="P20" t="s" s="63">
         <v>274</v>
       </c>
-      <c r="Q20" t="s" s="59">
+      <c r="Q20" t="s" s="63">
         <v>275</v>
       </c>
-      <c r="R20" t="s" s="59">
+      <c r="R20" t="s" s="63">
         <v>276</v>
       </c>
-      <c r="S20" t="s" s="59">
-        <v>35</v>
-      </c>
-      <c r="T20" t="s" s="59">
-        <v>35</v>
-      </c>
-      <c r="U20" t="s" s="59">
+      <c r="S20" t="s" s="63">
+        <v>35</v>
+      </c>
+      <c r="T20" t="s" s="63">
+        <v>35</v>
+      </c>
+      <c r="U20" t="s" s="63">
         <v>35</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s" s="61">
+      <c r="A21" t="s" s="65">
         <v>21</v>
       </c>
-      <c r="B21" t="s" s="61">
+      <c r="B21" t="s" s="65">
         <v>277</v>
       </c>
-      <c r="C21" t="s" s="61">
+      <c r="C21" t="s" s="65">
         <v>284</v>
       </c>
-      <c r="D21" t="s" s="61">
+      <c r="D21" t="s" s="65">
         <v>285</v>
       </c>
-      <c r="E21" t="s" s="62">
+      <c r="E21" t="s" s="66">
         <v>278</v>
       </c>
-      <c r="F21" t="s" s="61">
+      <c r="F21" t="s" s="65">
         <v>279</v>
       </c>
-      <c r="G21" t="s" s="61">
+      <c r="G21" t="s" s="65">
         <v>286</v>
       </c>
-      <c r="H21" t="s" s="61">
+      <c r="H21" t="s" s="65">
         <v>287</v>
       </c>
-      <c r="I21" t="n" s="119">
+      <c r="I21" t="n" s="123">
         <v>271.0</v>
       </c>
-      <c r="J21" t="s" s="61">
+      <c r="J21" t="s" s="65">
         <v>280</v>
       </c>
-      <c r="K21" t="s" s="120">
+      <c r="K21" t="s" s="124">
         <v>281</v>
       </c>
-      <c r="L21" t="s" s="61">
+      <c r="L21" t="s" s="65">
         <v>282</v>
       </c>
-      <c r="M21" t="s" s="61">
+      <c r="M21" t="s" s="65">
         <v>43</v>
       </c>
-      <c r="N21" t="s" s="61">
+      <c r="N21" t="s" s="65">
         <v>283</v>
       </c>
-      <c r="O21" s="61"/>
-      <c r="P21" t="s" s="61">
+      <c r="O21" s="65"/>
+      <c r="P21" t="s" s="65">
         <v>288</v>
       </c>
-      <c r="Q21" t="s" s="61">
-        <v>35</v>
-      </c>
-      <c r="R21" t="s" s="61">
+      <c r="Q21" t="s" s="65">
+        <v>35</v>
+      </c>
+      <c r="R21" t="s" s="65">
         <v>289</v>
       </c>
-      <c r="S21" t="s" s="61">
-        <v>35</v>
-      </c>
-      <c r="T21" t="s" s="61">
-        <v>35</v>
-      </c>
-      <c r="U21" t="s" s="61">
+      <c r="S21" t="s" s="65">
+        <v>35</v>
+      </c>
+      <c r="T21" t="s" s="65">
+        <v>35</v>
+      </c>
+      <c r="U21" t="s" s="65">
         <v>35</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s" s="63">
+      <c r="A22" t="s" s="67">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="63">
+      <c r="B22" t="s" s="67">
         <v>290</v>
       </c>
-      <c r="C22" t="s" s="63">
+      <c r="C22" t="s" s="67">
         <v>297</v>
       </c>
-      <c r="D22" t="s" s="63">
+      <c r="D22" t="s" s="67">
         <v>298</v>
       </c>
-      <c r="E22" t="s" s="64">
+      <c r="E22" t="s" s="68">
         <v>291</v>
       </c>
-      <c r="F22" t="s" s="63">
+      <c r="F22" t="s" s="67">
         <v>292</v>
       </c>
-      <c r="G22" t="s" s="63">
+      <c r="G22" t="s" s="67">
         <v>299</v>
       </c>
-      <c r="H22" t="s" s="63">
+      <c r="H22" t="s" s="67">
         <v>300</v>
       </c>
-      <c r="I22" t="n" s="121">
+      <c r="I22" t="n" s="125">
         <v>333.0</v>
       </c>
-      <c r="J22" t="s" s="63">
+      <c r="J22" t="s" s="67">
         <v>86</v>
       </c>
-      <c r="K22" t="s" s="122">
+      <c r="K22" t="s" s="126">
         <v>293</v>
       </c>
-      <c r="L22" t="s" s="63">
+      <c r="L22" t="s" s="67">
         <v>294</v>
       </c>
-      <c r="M22" t="s" s="63">
+      <c r="M22" t="s" s="67">
         <v>295</v>
       </c>
-      <c r="N22" t="s" s="63">
+      <c r="N22" t="s" s="67">
         <v>296</v>
       </c>
-      <c r="O22" s="63"/>
-      <c r="P22" t="s" s="63">
+      <c r="O22" s="67"/>
+      <c r="P22" t="s" s="67">
         <v>301</v>
       </c>
-      <c r="Q22" t="s" s="63">
+      <c r="Q22" t="s" s="67">
         <v>302</v>
       </c>
-      <c r="R22" t="s" s="63">
+      <c r="R22" t="s" s="67">
         <v>303</v>
       </c>
-      <c r="S22" t="s" s="63">
-        <v>35</v>
-      </c>
-      <c r="T22" t="s" s="63">
+      <c r="S22" t="s" s="67">
+        <v>35</v>
+      </c>
+      <c r="T22" t="s" s="67">
         <v>304</v>
       </c>
-      <c r="U22" t="s" s="63">
+      <c r="U22" t="s" s="67">
         <v>35</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s" s="65">
+      <c r="A23" t="s" s="69">
         <v>21</v>
       </c>
-      <c r="B23" t="s" s="65">
+      <c r="B23" t="s" s="69">
         <v>305</v>
       </c>
-      <c r="C23" t="s" s="65">
+      <c r="C23" t="s" s="69">
         <v>117</v>
       </c>
-      <c r="D23" t="s" s="65">
+      <c r="D23" t="s" s="69">
         <v>46</v>
       </c>
-      <c r="E23" t="s" s="66">
+      <c r="E23" t="s" s="70">
         <v>306</v>
       </c>
-      <c r="F23" t="s" s="65">
+      <c r="F23" t="s" s="69">
         <v>307</v>
       </c>
-      <c r="G23" t="s" s="65">
+      <c r="G23" t="s" s="69">
         <v>310</v>
       </c>
-      <c r="H23" t="s" s="65">
+      <c r="H23" t="s" s="69">
         <v>311</v>
       </c>
-      <c r="I23" t="n" s="123">
+      <c r="I23" t="n" s="127">
         <v>185.0</v>
       </c>
-      <c r="J23" t="s" s="65">
+      <c r="J23" t="s" s="69">
         <v>149</v>
       </c>
-      <c r="K23" t="s" s="124">
+      <c r="K23" t="s" s="128">
         <v>308</v>
       </c>
-      <c r="L23" t="s" s="65">
+      <c r="L23" t="s" s="69">
         <v>192</v>
       </c>
-      <c r="M23" t="s" s="65">
+      <c r="M23" t="s" s="69">
         <v>268</v>
       </c>
-      <c r="N23" t="s" s="65">
+      <c r="N23" t="s" s="69">
         <v>309</v>
       </c>
-      <c r="O23" s="65"/>
-      <c r="P23" t="s" s="65">
+      <c r="O23" s="69"/>
+      <c r="P23" t="s" s="69">
         <v>312</v>
       </c>
-      <c r="Q23" t="s" s="65">
+      <c r="Q23" t="s" s="69">
         <v>313</v>
       </c>
-      <c r="R23" t="s" s="65">
+      <c r="R23" t="s" s="69">
         <v>314</v>
       </c>
-      <c r="S23" t="s" s="65">
-        <v>35</v>
-      </c>
-      <c r="T23" t="s" s="65">
+      <c r="S23" t="s" s="69">
+        <v>35</v>
+      </c>
+      <c r="T23" t="s" s="69">
         <v>315</v>
       </c>
-      <c r="U23" t="s" s="65">
+      <c r="U23" t="s" s="69">
         <v>35</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s" s="67">
+      <c r="A24" t="s" s="71">
         <v>21</v>
       </c>
-      <c r="B24" t="s" s="67">
+      <c r="B24" t="s" s="71">
         <v>316</v>
       </c>
-      <c r="C24" t="s" s="67">
+      <c r="C24" t="s" s="71">
         <v>322</v>
       </c>
-      <c r="D24" t="s" s="67">
+      <c r="D24" t="s" s="71">
         <v>248</v>
       </c>
-      <c r="E24" t="s" s="68">
+      <c r="E24" t="s" s="72">
         <v>317</v>
       </c>
-      <c r="F24" t="s" s="67">
+      <c r="F24" t="s" s="71">
         <v>318</v>
       </c>
-      <c r="G24" t="s" s="67">
+      <c r="G24" t="s" s="71">
         <v>323</v>
       </c>
-      <c r="H24" t="s" s="67">
+      <c r="H24" t="s" s="71">
         <v>324</v>
       </c>
-      <c r="I24" t="n" s="125">
+      <c r="I24" t="n" s="129">
         <v>409.0</v>
       </c>
-      <c r="J24" t="s" s="67">
+      <c r="J24" t="s" s="71">
         <v>231</v>
       </c>
-      <c r="K24" t="s" s="126">
+      <c r="K24" t="s" s="130">
         <v>319</v>
       </c>
-      <c r="L24" t="s" s="67">
+      <c r="L24" t="s" s="71">
         <v>233</v>
       </c>
-      <c r="M24" t="s" s="67">
+      <c r="M24" t="s" s="71">
         <v>320</v>
       </c>
-      <c r="N24" t="s" s="67">
+      <c r="N24" t="s" s="71">
         <v>321</v>
       </c>
-      <c r="O24" s="67"/>
-      <c r="P24" t="s" s="67">
+      <c r="O24" s="71"/>
+      <c r="P24" t="s" s="71">
         <v>325</v>
       </c>
-      <c r="Q24" t="s" s="67">
+      <c r="Q24" t="s" s="71">
         <v>326</v>
       </c>
-      <c r="R24" t="s" s="67">
+      <c r="R24" t="s" s="71">
         <v>314</v>
       </c>
-      <c r="S24" t="s" s="67">
-        <v>35</v>
-      </c>
-      <c r="T24" t="s" s="67">
-        <v>35</v>
-      </c>
-      <c r="U24" t="s" s="67">
+      <c r="S24" t="s" s="71">
+        <v>35</v>
+      </c>
+      <c r="T24" t="s" s="71">
+        <v>35</v>
+      </c>
+      <c r="U24" t="s" s="71">
         <v>35</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s" s="69">
+      <c r="A25" t="s" s="73">
         <v>21</v>
       </c>
-      <c r="B25" t="s" s="69">
+      <c r="B25" t="s" s="73">
         <v>327</v>
       </c>
-      <c r="C25" t="s" s="69">
+      <c r="C25" t="s" s="73">
         <v>322</v>
       </c>
-      <c r="D25" t="s" s="69">
+      <c r="D25" t="s" s="73">
         <v>334</v>
       </c>
-      <c r="E25" t="s" s="70">
+      <c r="E25" t="s" s="74">
         <v>328</v>
       </c>
-      <c r="F25" t="s" s="69">
+      <c r="F25" t="s" s="73">
         <v>329</v>
       </c>
-      <c r="G25" t="s" s="69">
+      <c r="G25" t="s" s="73">
         <v>335</v>
       </c>
-      <c r="H25" t="s" s="69">
+      <c r="H25" t="s" s="73">
         <v>336</v>
       </c>
-      <c r="I25" t="n" s="127">
+      <c r="I25" t="n" s="131">
         <v>248.0</v>
       </c>
-      <c r="J25" t="s" s="69">
+      <c r="J25" t="s" s="73">
         <v>330</v>
       </c>
-      <c r="K25" t="s" s="128">
+      <c r="K25" t="s" s="132">
         <v>331</v>
       </c>
-      <c r="L25" t="s" s="69">
+      <c r="L25" t="s" s="73">
         <v>332</v>
       </c>
-      <c r="M25" t="s" s="69">
+      <c r="M25" t="s" s="73">
         <v>181</v>
       </c>
-      <c r="N25" t="s" s="69">
+      <c r="N25" t="s" s="73">
         <v>333</v>
       </c>
-      <c r="O25" s="69"/>
-      <c r="P25" t="s" s="69">
+      <c r="O25" s="73"/>
+      <c r="P25" t="s" s="73">
         <v>337</v>
       </c>
-      <c r="Q25" t="s" s="69">
+      <c r="Q25" t="s" s="73">
         <v>50</v>
       </c>
-      <c r="R25" t="s" s="69">
+      <c r="R25" t="s" s="73">
         <v>276</v>
       </c>
-      <c r="S25" t="s" s="69">
-        <v>35</v>
-      </c>
-      <c r="T25" t="s" s="69">
-        <v>35</v>
-      </c>
-      <c r="U25" t="s" s="69">
+      <c r="S25" t="s" s="73">
+        <v>35</v>
+      </c>
+      <c r="T25" t="s" s="73">
+        <v>35</v>
+      </c>
+      <c r="U25" t="s" s="73">
         <v>35</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s" s="71">
+      <c r="A26" t="s" s="75">
         <v>21</v>
       </c>
-      <c r="B26" t="s" s="71">
+      <c r="B26" t="s" s="75">
         <v>338</v>
       </c>
-      <c r="C26" t="s" s="71">
+      <c r="C26" t="s" s="75">
         <v>345</v>
       </c>
-      <c r="D26" t="s" s="71">
+      <c r="D26" t="s" s="75">
         <v>76</v>
       </c>
-      <c r="E26" t="s" s="72">
+      <c r="E26" t="s" s="76">
         <v>30</v>
       </c>
-      <c r="F26" t="s" s="71">
+      <c r="F26" t="s" s="75">
         <v>339</v>
       </c>
-      <c r="G26" t="s" s="71">
+      <c r="G26" t="s" s="75">
         <v>346</v>
       </c>
-      <c r="H26" t="s" s="71">
+      <c r="H26" t="s" s="75">
         <v>347</v>
       </c>
-      <c r="I26" t="n" s="129">
+      <c r="I26" t="n" s="133">
         <v>424.0</v>
       </c>
-      <c r="J26" t="s" s="71">
+      <c r="J26" t="s" s="75">
         <v>340</v>
       </c>
-      <c r="K26" t="s" s="130">
+      <c r="K26" t="s" s="134">
         <v>341</v>
       </c>
-      <c r="L26" t="s" s="71">
+      <c r="L26" t="s" s="75">
         <v>342</v>
       </c>
-      <c r="M26" t="s" s="71">
+      <c r="M26" t="s" s="75">
         <v>343</v>
       </c>
-      <c r="N26" t="s" s="71">
+      <c r="N26" t="s" s="75">
         <v>344</v>
       </c>
-      <c r="O26" s="71"/>
-      <c r="P26" t="s" s="71">
+      <c r="O26" s="75"/>
+      <c r="P26" t="s" s="75">
         <v>348</v>
       </c>
-      <c r="Q26" t="s" s="71">
+      <c r="Q26" t="s" s="75">
         <v>349</v>
       </c>
-      <c r="R26" t="s" s="71">
+      <c r="R26" t="s" s="75">
         <v>350</v>
       </c>
-      <c r="S26" t="s" s="71">
-        <v>35</v>
-      </c>
-      <c r="T26" t="s" s="71">
+      <c r="S26" t="s" s="75">
+        <v>35</v>
+      </c>
+      <c r="T26" t="s" s="75">
         <v>52</v>
       </c>
-      <c r="U26" t="s" s="71">
+      <c r="U26" t="s" s="75">
         <v>35</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="73">
+      <c r="A27" t="s" s="77">
         <v>21</v>
       </c>
-      <c r="B27" t="s" s="73">
+      <c r="B27" t="s" s="77">
         <v>351</v>
       </c>
-      <c r="C27" t="s" s="73">
+      <c r="C27" t="s" s="77">
         <v>359</v>
       </c>
-      <c r="D27" t="s" s="73">
+      <c r="D27" t="s" s="77">
         <v>271</v>
       </c>
-      <c r="E27" t="s" s="74">
+      <c r="E27" t="s" s="78">
         <v>352</v>
       </c>
-      <c r="F27" t="s" s="73">
+      <c r="F27" t="s" s="77">
         <v>353</v>
       </c>
-      <c r="G27" t="s" s="73">
+      <c r="G27" t="s" s="77">
         <v>360</v>
       </c>
-      <c r="H27" t="s" s="73">
+      <c r="H27" t="s" s="77">
         <v>361</v>
       </c>
-      <c r="I27" t="n" s="131">
+      <c r="I27" t="n" s="135">
         <v>259.0</v>
       </c>
-      <c r="J27" t="s" s="73">
+      <c r="J27" t="s" s="77">
         <v>354</v>
       </c>
-      <c r="K27" t="s" s="132">
+      <c r="K27" t="s" s="136">
         <v>355</v>
       </c>
-      <c r="L27" t="s" s="73">
+      <c r="L27" t="s" s="77">
         <v>356</v>
       </c>
-      <c r="M27" t="s" s="73">
+      <c r="M27" t="s" s="77">
         <v>357</v>
       </c>
-      <c r="N27" t="s" s="73">
+      <c r="N27" t="s" s="77">
         <v>358</v>
       </c>
-      <c r="O27" s="73"/>
-      <c r="P27" t="s" s="73">
+      <c r="O27" s="77"/>
+      <c r="P27" t="s" s="77">
         <v>362</v>
       </c>
-      <c r="Q27" t="s" s="73">
+      <c r="Q27" t="s" s="77">
         <v>363</v>
       </c>
-      <c r="R27" t="s" s="73">
+      <c r="R27" t="s" s="77">
         <v>364</v>
       </c>
-      <c r="S27" t="s" s="73">
+      <c r="S27" t="s" s="77">
         <v>365</v>
       </c>
-      <c r="T27" t="s" s="73">
+      <c r="T27" t="s" s="77">
         <v>366</v>
       </c>
-      <c r="U27" t="s" s="73">
+      <c r="U27" t="s" s="77">
         <v>35</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s" s="75">
+      <c r="A28" t="s" s="79">
         <v>21</v>
       </c>
-      <c r="B28" t="s" s="75">
+      <c r="B28" t="s" s="79">
         <v>367</v>
       </c>
-      <c r="C28" t="s" s="75">
+      <c r="C28" t="s" s="79">
         <v>284</v>
       </c>
-      <c r="D28" t="s" s="75">
+      <c r="D28" t="s" s="79">
         <v>140</v>
       </c>
-      <c r="E28" t="s" s="76">
+      <c r="E28" t="s" s="80">
         <v>368</v>
       </c>
-      <c r="F28" t="s" s="75">
+      <c r="F28" t="s" s="79">
         <v>369</v>
       </c>
-      <c r="G28" t="s" s="75">
+      <c r="G28" t="s" s="79">
         <v>373</v>
       </c>
-      <c r="H28" t="s" s="75">
+      <c r="H28" t="s" s="79">
         <v>374</v>
       </c>
-      <c r="I28" t="n" s="133">
+      <c r="I28" t="n" s="137">
         <v>306.0</v>
       </c>
-      <c r="J28" t="s" s="75">
+      <c r="J28" t="s" s="79">
         <v>192</v>
       </c>
-      <c r="K28" t="s" s="134">
+      <c r="K28" t="s" s="138">
         <v>370</v>
       </c>
-      <c r="L28" t="s" s="75">
+      <c r="L28" t="s" s="79">
         <v>371</v>
       </c>
-      <c r="M28" t="s" s="75">
+      <c r="M28" t="s" s="79">
         <v>43</v>
       </c>
-      <c r="N28" t="s" s="75">
+      <c r="N28" t="s" s="79">
         <v>372</v>
       </c>
-      <c r="O28" s="75"/>
-      <c r="P28" t="s" s="75">
+      <c r="O28" s="79"/>
+      <c r="P28" t="s" s="79">
         <v>375</v>
       </c>
-      <c r="Q28" t="s" s="75">
+      <c r="Q28" t="s" s="79">
         <v>376</v>
       </c>
-      <c r="R28" t="s" s="75">
+      <c r="R28" t="s" s="79">
         <v>377</v>
       </c>
-      <c r="S28" t="s" s="75">
-        <v>35</v>
-      </c>
-      <c r="T28" t="s" s="75">
+      <c r="S28" t="s" s="79">
+        <v>35</v>
+      </c>
+      <c r="T28" t="s" s="79">
         <v>378</v>
       </c>
-      <c r="U28" t="s" s="75">
+      <c r="U28" t="s" s="79">
         <v>35</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s" s="77">
+      <c r="A29" t="s" s="81">
         <v>21</v>
       </c>
-      <c r="B29" t="s" s="77">
+      <c r="B29" t="s" s="81">
         <v>379</v>
       </c>
-      <c r="C29" t="s" s="77">
+      <c r="C29" t="s" s="81">
         <v>387</v>
       </c>
-      <c r="D29" t="s" s="77">
+      <c r="D29" t="s" s="81">
         <v>388</v>
       </c>
-      <c r="E29" t="s" s="78">
+      <c r="E29" t="s" s="82">
         <v>380</v>
       </c>
-      <c r="F29" t="s" s="77">
+      <c r="F29" t="s" s="81">
         <v>381</v>
       </c>
-      <c r="G29" t="s" s="77">
+      <c r="G29" t="s" s="81">
         <v>389</v>
       </c>
-      <c r="H29" t="s" s="77">
+      <c r="H29" t="s" s="81">
         <v>390</v>
       </c>
-      <c r="I29" t="n" s="135">
+      <c r="I29" t="n" s="139">
         <v>587.0</v>
       </c>
-      <c r="J29" t="s" s="77">
+      <c r="J29" t="s" s="81">
         <v>382</v>
       </c>
-      <c r="K29" t="s" s="136">
+      <c r="K29" t="s" s="140">
         <v>383</v>
       </c>
-      <c r="L29" t="s" s="77">
+      <c r="L29" t="s" s="81">
         <v>384</v>
       </c>
-      <c r="M29" t="s" s="77">
+      <c r="M29" t="s" s="81">
         <v>385</v>
       </c>
-      <c r="N29" t="s" s="77">
+      <c r="N29" t="s" s="81">
         <v>386</v>
       </c>
-      <c r="O29" s="77"/>
-      <c r="P29" t="s" s="77">
+      <c r="O29" s="81"/>
+      <c r="P29" t="s" s="81">
         <v>391</v>
       </c>
-      <c r="Q29" t="s" s="77">
+      <c r="Q29" t="s" s="81">
         <v>392</v>
       </c>
-      <c r="R29" t="s" s="77">
+      <c r="R29" t="s" s="81">
         <v>393</v>
       </c>
-      <c r="S29" t="s" s="77">
-        <v>35</v>
-      </c>
-      <c r="T29" t="s" s="77">
+      <c r="S29" t="s" s="81">
+        <v>35</v>
+      </c>
+      <c r="T29" t="s" s="81">
         <v>394</v>
       </c>
-      <c r="U29" t="s" s="77">
+      <c r="U29" t="s" s="81">
         <v>35</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s" s="79">
+      <c r="A30" t="s" s="83">
         <v>21</v>
       </c>
-      <c r="B30" t="s" s="79">
+      <c r="B30" t="s" s="83">
         <v>395</v>
       </c>
-      <c r="C30" t="s" s="79">
+      <c r="C30" t="s" s="83">
         <v>401</v>
       </c>
-      <c r="D30" t="s" s="79">
+      <c r="D30" t="s" s="83">
         <v>381</v>
       </c>
-      <c r="E30" t="s" s="80">
+      <c r="E30" t="s" s="84">
         <v>396</v>
       </c>
-      <c r="F30" t="s" s="79">
+      <c r="F30" t="s" s="83">
         <v>397</v>
       </c>
-      <c r="G30" t="s" s="79">
+      <c r="G30" t="s" s="83">
         <v>402</v>
       </c>
-      <c r="H30" t="s" s="79">
+      <c r="H30" t="s" s="83">
         <v>403</v>
       </c>
-      <c r="I30" t="n" s="137">
+      <c r="I30" t="n" s="141">
         <v>134.0</v>
       </c>
-      <c r="J30" t="s" s="79">
+      <c r="J30" t="s" s="83">
         <v>398</v>
       </c>
-      <c r="K30" t="s" s="138">
+      <c r="K30" t="s" s="142">
         <v>399</v>
       </c>
-      <c r="L30" t="s" s="79">
+      <c r="L30" t="s" s="83">
         <v>280</v>
       </c>
-      <c r="M30" t="s" s="79">
+      <c r="M30" t="s" s="83">
         <v>219</v>
       </c>
-      <c r="N30" t="s" s="79">
+      <c r="N30" t="s" s="83">
         <v>400</v>
       </c>
-      <c r="O30" s="79"/>
-      <c r="P30" t="s" s="79">
+      <c r="O30" s="83"/>
+      <c r="P30" t="s" s="83">
         <v>404</v>
       </c>
-      <c r="Q30" t="s" s="79">
+      <c r="Q30" t="s" s="83">
         <v>405</v>
       </c>
-      <c r="R30" t="s" s="79">
+      <c r="R30" t="s" s="83">
         <v>406</v>
       </c>
-      <c r="S30" t="s" s="79">
-        <v>35</v>
-      </c>
-      <c r="T30" t="s" s="79">
+      <c r="S30" t="s" s="83">
+        <v>35</v>
+      </c>
+      <c r="T30" t="s" s="83">
         <v>407</v>
       </c>
-      <c r="U30" t="s" s="79">
+      <c r="U30" t="s" s="83">
         <v>35</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s" s="1">
+      <c r="A32" t="s" s="5">
         <v>408</v>
       </c>
-      <c r="B32" t="n" s="1">
+      <c r="B32" t="n" s="5">
         <v>29.0</v>
       </c>
-      <c r="C32" t="s" s="1">
+      <c r="C32" t="s" s="5">
         <v>409</v>
       </c>
-      <c r="D32" t="s" s="1">
+      <c r="D32" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="E32" t="s" s="1">
+      <c r="E32" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="F32" t="s" s="1">
+      <c r="F32" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="G32" t="s" s="1">
+      <c r="G32" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="H32" t="s" s="1">
+      <c r="H32" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="I32" t="n" s="1">
+      <c r="I32" t="n" s="5">
         <v>8140.0</v>
       </c>
-      <c r="J32" t="n" s="1">
+      <c r="J32" t="n" s="5">
         <v>1069.0</v>
       </c>
-      <c r="K32" t="s" s="1">
+      <c r="K32" t="s" s="5">
         <v>410</v>
       </c>
-      <c r="L32" t="n" s="1">
+      <c r="L32" t="n" s="5">
         <v>1801.0</v>
       </c>
-      <c r="M32" t="s" s="1">
+      <c r="M32" t="s" s="5">
         <v>411</v>
       </c>
-      <c r="N32" t="s" s="1">
+      <c r="N32" t="s" s="5">
         <v>412</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s" s="1">
+      <c r="A33" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="B33" t="s" s="1">
+      <c r="B33" t="s" s="5">
         <v>413</v>
       </c>
-      <c r="C33" t="s" s="1">
+      <c r="C33" t="s" s="5">
         <v>414</v>
       </c>
-      <c r="D33" t="s" s="1">
+      <c r="D33" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="E33" t="s" s="1">
+      <c r="E33" t="s" s="5">
         <v>413</v>
       </c>
-      <c r="F33" t="s" s="1">
+      <c r="F33" t="s" s="5">
         <v>413</v>
       </c>
-      <c r="H33" t="n" s="1">
+      <c r="H33" t="n" s="5">
         <v>281.0</v>
       </c>
-      <c r="I33" t="n" s="1">
+      <c r="I33" t="n" s="5">
         <v>281.0</v>
       </c>
-      <c r="J33" t="s" s="1">
+      <c r="J33" t="s" s="5">
         <v>71</v>
       </c>
-      <c r="K33" t="s" s="1">
+      <c r="K33" t="s" s="5">
         <v>415</v>
       </c>
-      <c r="L33" t="s" s="1">
+      <c r="L33" t="s" s="5">
         <v>165</v>
       </c>
-      <c r="M33" t="s" s="1">
+      <c r="M33" t="s" s="5">
         <v>357</v>
       </c>
-      <c r="N33" t="s" s="1">
+      <c r="N33" t="s" s="5">
         <v>372</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="5">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="F37" t="s" s="2">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="B38" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E38" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s" s="2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="B39" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E39" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="F39" t="s" s="2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="B40" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E40" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="F40" t="s" s="2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="B41" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E41" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s" s="2">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="B42" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="F42" t="s" s="2">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="B43" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="F43" t="s" s="2">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="B44" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s" s="2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="B45" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C45" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E45" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="F45" t="s" s="2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="B46" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="D46" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="E46" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="F46" t="s" s="2">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="5">
+        <v>439</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="16">
     <mergeCell ref="A32:A33"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="C32:H32"/>
     <mergeCell ref="C33:H33"/>
+    <mergeCell ref="A36:F36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A47:F47"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>